<commit_message>
prototype for grouped bar chart
</commit_message>
<xml_diff>
--- a/data/SampleScreeningData.xlsx
+++ b/data/SampleScreeningData.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="check" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Agency</t>
   </si>
@@ -503,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -2188,4 +2189,1695 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q35"/>
+  <sheetViews>
+    <sheetView topLeftCell="K25" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>11</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>27</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>6</v>
+      </c>
+      <c r="Q2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>24</v>
+      </c>
+      <c r="Q6">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>43</v>
+      </c>
+      <c r="L7">
+        <v>2</v>
+      </c>
+      <c r="M7">
+        <v>16</v>
+      </c>
+      <c r="N7">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>8</v>
+      </c>
+      <c r="P7">
+        <v>18</v>
+      </c>
+      <c r="Q7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>12</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>21</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>15</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>14</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+      <c r="Q10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13">
+        <v>35</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>58</v>
+      </c>
+      <c r="E13">
+        <v>35</v>
+      </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>62</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>25</v>
+      </c>
+      <c r="N13">
+        <v>8</v>
+      </c>
+      <c r="O13">
+        <v>17</v>
+      </c>
+      <c r="P13">
+        <v>9</v>
+      </c>
+      <c r="Q13">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <v>30</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>11</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>47</v>
+      </c>
+      <c r="L15">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>24</v>
+      </c>
+      <c r="N15">
+        <v>22</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <v>12</v>
+      </c>
+      <c r="Q15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>34</v>
+      </c>
+      <c r="E16">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>8</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+      <c r="K16">
+        <v>41</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>20</v>
+      </c>
+      <c r="N16">
+        <v>13</v>
+      </c>
+      <c r="O16">
+        <v>22</v>
+      </c>
+      <c r="P16">
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>28</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>11</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>14</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>2</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>45</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>11</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>13</v>
+      </c>
+      <c r="P19">
+        <v>54</v>
+      </c>
+      <c r="Q19">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+      <c r="N20">
+        <v>9</v>
+      </c>
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>4</v>
+      </c>
+      <c r="O21">
+        <v>2</v>
+      </c>
+      <c r="P21">
+        <v>6</v>
+      </c>
+      <c r="Q21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>23</v>
+      </c>
+      <c r="E22">
+        <v>10</v>
+      </c>
+      <c r="F22">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>30</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>14</v>
+      </c>
+      <c r="N22">
+        <v>8</v>
+      </c>
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>12</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>3</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>3</v>
+      </c>
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>8</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+      <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>18</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>9</v>
+      </c>
+      <c r="N25">
+        <v>9</v>
+      </c>
+      <c r="O25">
+        <v>9</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
+      <c r="Q25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
+      <c r="O27">
+        <v>2</v>
+      </c>
+      <c r="P27">
+        <v>14</v>
+      </c>
+      <c r="Q27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>4</v>
+      </c>
+      <c r="Q28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29">
+        <v>57</v>
+      </c>
+      <c r="E29">
+        <v>41</v>
+      </c>
+      <c r="F29">
+        <v>29</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29">
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>95</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>22</v>
+      </c>
+      <c r="N29">
+        <v>9</v>
+      </c>
+      <c r="O29">
+        <v>20</v>
+      </c>
+      <c r="P29">
+        <v>64</v>
+      </c>
+      <c r="Q29">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>21</v>
+      </c>
+      <c r="D30">
+        <v>36</v>
+      </c>
+      <c r="E30">
+        <v>28</v>
+      </c>
+      <c r="F30">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>18</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>45</v>
+      </c>
+      <c r="L30">
+        <v>3</v>
+      </c>
+      <c r="M30">
+        <v>32</v>
+      </c>
+      <c r="N30">
+        <v>17</v>
+      </c>
+      <c r="O30">
+        <v>26</v>
+      </c>
+      <c r="P30">
+        <v>26</v>
+      </c>
+      <c r="Q30">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1">
+        <f>SUM(B2:B30)</f>
+        <v>243</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" ref="C31:Q31" si="0">SUM(C2:C30)</f>
+        <v>123</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>429</v>
+      </c>
+      <c r="E31" s="1">
+        <f t="shared" si="0"/>
+        <v>238</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>294</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>616</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="0"/>
+        <v>244</v>
+      </c>
+      <c r="N31" s="1">
+        <f t="shared" si="0"/>
+        <v>152</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="0"/>
+        <v>209</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="Q31" s="1">
+        <f t="shared" si="0"/>
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>7</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>19</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <v>13</v>
+      </c>
+      <c r="I35">
+        <v>5</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>18</v>
+      </c>
+      <c r="L35">
+        <v>5</v>
+      </c>
+      <c r="M35">
+        <v>10</v>
+      </c>
+      <c r="N35">
+        <v>4</v>
+      </c>
+      <c r="O35">
+        <v>16</v>
+      </c>
+      <c r="P35">
+        <v>4</v>
+      </c>
+      <c r="Q35">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>